<commit_message>
Added video lecture 4
</commit_message>
<xml_diff>
--- a/docs/file-api-browsers.xlsx
+++ b/docs/file-api-browsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26160" windowHeight="16320" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="80" windowWidth="25040" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Blob response type</t>
   </si>
   <si>
-    <t>Firefox Android 10</t>
-  </si>
-  <si>
     <t>iOS 5</t>
   </si>
   <si>
@@ -90,7 +87,10 @@
     <t>Chrome 17</t>
   </si>
   <si>
-    <t>Firefox 10</t>
+    <t>Firefox 11</t>
+  </si>
+  <si>
+    <t>Firefox Android 11</t>
   </si>
 </sst>
 </file>
@@ -304,8 +304,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,7 +470,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -501,6 +507,9 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -537,6 +546,9 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -869,7 +881,7 @@
   <dimension ref="A7:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="H20" sqref="A7:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -887,25 +899,25 @@
     <row r="7" spans="1:8" ht="41" thickBot="1">
       <c r="A7" s="1"/>
       <c r="B7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>7</v>
-      </c>
       <c r="F7" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="23">
@@ -925,25 +937,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="21" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="20">
@@ -951,25 +963,25 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="20">
@@ -977,25 +989,25 @@
         <v>3</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="20">
@@ -1003,25 +1015,25 @@
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20">
@@ -1029,30 +1041,30 @@
         <v>5</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="23">
       <c r="A14" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
@@ -1064,59 +1076,59 @@
     </row>
     <row r="15" spans="1:8" ht="20">
       <c r="A15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20">
       <c r="A16" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="23">
       <c r="A17" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
@@ -1128,33 +1140,33 @@
     </row>
     <row r="18" spans="1:8" ht="31">
       <c r="A18" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>21</v>
-      </c>
       <c r="E18" s="26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>